<commit_message>
Modify sheet name sales_records
</commit_message>
<xml_diff>
--- a/files/100_Sales_Records.xlsx
+++ b/files/100_Sales_Records.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Wayyenlin/Code/GitHubCode/pycon2019-pyexcel/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1681C46-FA18-6C4E-AF6B-48AAFCD31A7F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2DE9C9-CBA6-5243-96AE-84CB87F7DC86}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="24960" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PVT" sheetId="2" r:id="rId1"/>
-    <sheet name="100_Sales_Records" sheetId="1" r:id="rId2"/>
+    <sheet name="sales_records" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="40" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -933,10 +933,2120 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[100_Sales_Records.xlsx]PVT!PVT</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baby Food</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$B$5:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Beverages</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$C$5:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cereal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$D$5:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Clothes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$E$5:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cosmetics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$F$5:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$G$3:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fruits</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$G$5:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$H$3:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Household</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$H$5:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$I$3:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$I$5:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$J$3:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Office Supplies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$J$5:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$K$3:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Personal Care</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$K$5:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$L$3:$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Snacks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$L$5:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$M$3:$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vegetables</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$M$5:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PVT!$N$3:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PVT!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Australia and Oceania</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Central America and the Caribbean</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europe</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Middle East and North Africa</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>North America</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sub-Saharan Africa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(blank)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PVT!$N$5:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-64FB-5D40-8B72-5B7A3A81EF1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1780508927"/>
+        <c:axId val="1780575855"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1780508927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1780575855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1780575855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1780508927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A29E229-E8C1-BB48-9503-0FD99D11BE7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="WayYen Lin" refreshedDate="43682.918898611111" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="101" xr:uid="{00000000-000A-0000-FFFF-FFFF12000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="WayYen Lin" refreshedDate="43721.807635879632" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="101" xr:uid="{00000000-000A-0000-FFFF-FFFF12000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:N1048576" sheet="100_Sales_Records"/>
+    <worksheetSource ref="A1:N1048576" sheet="sales_records"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="Region" numFmtId="0">
@@ -2635,7 +4745,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PVT" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PVT" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:O13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" showAll="0">
@@ -2764,6 +4874,164 @@
   <dataFields count="1">
     <dataField name="Count of Item Type" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="13">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3075,7 +5343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3463,6 +5731,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3470,7 +5739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>